<commit_message>
fistosi ci siamo quasi :)
</commit_message>
<xml_diff>
--- a/xls/foscarini/result/foscarini_aumentato.xlsx
+++ b/xls/foscarini/result/foscarini_aumentato.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17165" count="17165">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16977" count="16977">
   <x:si>
     <x:t>supplier</x:t>
   </x:si>
@@ -38,9 +38,6 @@
   </x:si>
   <x:si>
     <x:t>ean13</x:t>
-  </x:si>
-  <x:si>
-    <x:t>price</x:t>
   </x:si>
   <x:si>
     <x:t>color</x:t>
@@ -86,6 +83,9 @@
   </x:si>
   <x:si>
     <x:t>pic</x:t>
+  </x:si>
+  <x:si>
+    <x:t>light_schema</x:t>
   </x:si>
   <x:si>
     <x:t>otherColors</x:t>

</xml_diff>